<commit_message>
QoL: parameter script calling from CMake
</commit_message>
<xml_diff>
--- a/parameter_database.xlsx
+++ b/parameter_database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="2689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="2688">
   <si>
     <t>On-Board Parameters</t>
   </si>
@@ -7573,7 +7573,7 @@
     <t>COMMS-001</t>
   </si>
   <si>
-    <t>uhf_power_amp_temp</t>
+    <t>UHF_POWER_AMP_TEMP</t>
   </si>
   <si>
     <t>UHF band PA temperature</t>
@@ -7582,7 +7582,7 @@
     <t>COMMS-002</t>
   </si>
   <si>
-    <t>pcb_temp</t>
+    <t>PCB_TEMP</t>
   </si>
   <si>
     <t>COMMS PCB temperature 1</t>
@@ -7591,7 +7591,7 @@
     <t>COMMS-003</t>
   </si>
   <si>
-    <t>gnss_temp</t>
+    <t>GNSS_TEMP</t>
   </si>
   <si>
     <t>COMMS PCB temperature 2</t>
@@ -7606,7 +7606,7 @@
     <t>COMMS-005</t>
   </si>
   <si>
-    <t>antenna_deployment_status</t>
+    <t>ANTENNA_DEPLOYMENT_STATUS</t>
   </si>
   <si>
     <t>Antenna deployment status</t>
@@ -7640,7 +7640,7 @@
     <t>COMMS-008</t>
   </si>
   <si>
-    <t>cw_interval</t>
+    <t>CW_INTERVAL</t>
   </si>
   <si>
     <t>CW Interval</t>
@@ -7649,7 +7649,7 @@
     <t>COMMS-009</t>
   </si>
   <si>
-    <t>bfsk_beacon_interval</t>
+    <t>BFSK_BEAKON_INTERVAL</t>
   </si>
   <si>
     <t>Gaussian BFSK Beacon Interval</t>
@@ -7658,7 +7658,7 @@
     <t>COMMS-010</t>
   </si>
   <si>
-    <t>uhf_tx_power</t>
+    <t>UHF_TX_POWER</t>
   </si>
   <si>
     <t xml:space="preserve">UHF band TX Power </t>
@@ -7700,7 +7700,7 @@
     <t>COMMS-015</t>
   </si>
   <si>
-    <t>rssi</t>
+    <t>RSSI</t>
   </si>
   <si>
     <t>Received signal strength indicator (RSSI)</t>
@@ -7808,7 +7808,7 @@
     <t>COMMS-031</t>
   </si>
   <si>
-    <t>gnss_lat</t>
+    <t>GNSS_LAT</t>
   </si>
   <si>
     <t>GNSS Position (Lat)</t>
@@ -7820,7 +7820,7 @@
     <t>COMMS-032</t>
   </si>
   <si>
-    <t>gnss_long</t>
+    <t>GNSS_LONG</t>
   </si>
   <si>
     <t>GNSS Position (Long)</t>
@@ -7829,7 +7829,7 @@
     <t>COMMS-033</t>
   </si>
   <si>
-    <t>gnss_alt</t>
+    <t>GNSS_ALT</t>
   </si>
   <si>
     <t>GNSS Position (Alt)</t>
@@ -7838,13 +7838,13 @@
     <t>COMMS-034</t>
   </si>
   <si>
-    <t>gnss_time</t>
+    <t>GNSS_TIME</t>
   </si>
   <si>
     <t>COMMS-035</t>
   </si>
   <si>
-    <t>gnss_ack_timeout</t>
+    <t>GNSS_ACK_TIMEOUT</t>
   </si>
   <si>
     <t>GNSS ACK Timeout for its response (ISR)</t>
@@ -7853,7 +7853,7 @@
     <t>COMMS-036</t>
   </si>
   <si>
-    <t>gnss_cmd_retries</t>
+    <t>GNSS_CMD_RETRIES</t>
   </si>
   <si>
     <t>How many retries have to be done for a command before an error is raised</t>
@@ -7862,7 +7862,7 @@
     <t>COMMS-037</t>
   </si>
   <si>
-    <t>gnss_error_timeout</t>
+    <t>GNSS_ERROR_TIMEOUT</t>
   </si>
   <si>
     <t>GNSS Error Timeout for the periodic message from the GNSS</t>
@@ -7871,7 +7871,7 @@
     <t>COMMS-038</t>
   </si>
   <si>
-    <t>error_timeout_cnt_thrhd</t>
+    <t>ERROR_TIMEOUT_CNT_THRHD</t>
   </si>
   <si>
     <t>Counter for the above error that resets the GNSS</t>
@@ -7880,7 +7880,7 @@
     <t>COMMS-039</t>
   </si>
   <si>
-    <t>gnss_delay_cmds</t>
+    <t>GNSS_DELAY_CMDS</t>
   </si>
   <si>
     <t>Delay between commands (must be above 100)</t>
@@ -7889,7 +7889,7 @@
     <t>COMMS-040</t>
   </si>
   <si>
-    <t>satellites_tracked</t>
+    <t>SATELLITES_TRACKED</t>
   </si>
   <si>
     <t>How many satellites are tracked</t>
@@ -7898,7 +7898,7 @@
     <t>COMMS-041</t>
   </si>
   <si>
-    <t>gnss_fix_quality</t>
+    <t>GNSS_FIX_QUALITY</t>
   </si>
   <si>
     <t>GNSS signal quality</t>
@@ -7907,7 +7907,7 @@
     <t>COMMS-042</t>
   </si>
   <si>
-    <t>gnss_TM_data_period</t>
+    <t>GNSS_TM_DATA_PERIOD</t>
   </si>
   <si>
     <t>Time between consecutive GNSS data</t>
@@ -7919,9 +7919,6 @@
     <t>COMMS-043</t>
   </si>
   <si>
-    <t>commit_hash</t>
-  </si>
-  <si>
     <t>COMMS Software commit hash</t>
   </si>
   <si>
@@ -8177,7 +8174,7 @@
     <t>COMMS-086</t>
   </si>
   <si>
-    <t>emmc_usage</t>
+    <t>EMMC_USAGE</t>
   </si>
   <si>
     <t>eMMC usage</t>
@@ -54131,14 +54128,14 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J4:J47 J49:J1249">
@@ -69376,7 +69373,7 @@
     <col customWidth="1" min="1" max="1" width="11.63"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
     <col customWidth="1" min="4" max="4" width="6.13"/>
-    <col customWidth="1" min="5" max="5" width="23.0"/>
+    <col customWidth="1" min="5" max="5" width="27.38"/>
     <col customWidth="1" min="6" max="6" width="34.38"/>
     <col customWidth="1" min="7" max="7" width="18.38"/>
     <col customWidth="1" min="8" max="10" width="14.25"/>
@@ -71234,16 +71231,16 @@
         <v>266</v>
       </c>
       <c r="C51" s="127" t="s">
-        <v>247</v>
+        <v>297</v>
       </c>
       <c r="D51" s="127">
         <v>1.0</v>
       </c>
       <c r="E51" s="127" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F51" s="128" t="s">
         <v>2601</v>
-      </c>
-      <c r="F51" s="128" t="s">
-        <v>2602</v>
       </c>
       <c r="G51" s="127"/>
       <c r="H51" s="127"/>
@@ -71269,10 +71266,10 @@
     </row>
     <row r="52">
       <c r="A52" s="261" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B52" s="127" t="s">
         <v>2603</v>
-      </c>
-      <c r="B52" s="127" t="s">
-        <v>2604</v>
       </c>
       <c r="C52" s="256" t="s">
         <v>1758</v>
@@ -71282,7 +71279,7 @@
       </c>
       <c r="E52" s="127"/>
       <c r="F52" s="128" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="G52" s="127"/>
       <c r="H52" s="127"/>
@@ -71308,10 +71305,10 @@
     </row>
     <row r="53">
       <c r="A53" s="261" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="B53" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C53" s="256" t="s">
         <v>1758</v>
@@ -71321,7 +71318,7 @@
       </c>
       <c r="E53" s="262"/>
       <c r="F53" s="128" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="G53" s="262"/>
       <c r="H53" s="262"/>
@@ -71347,10 +71344,10 @@
     </row>
     <row r="54">
       <c r="A54" s="261" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="B54" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C54" s="256" t="s">
         <v>1758</v>
@@ -71360,7 +71357,7 @@
       </c>
       <c r="E54" s="262"/>
       <c r="F54" s="128" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="G54" s="262"/>
       <c r="H54" s="262"/>
@@ -71386,10 +71383,10 @@
     </row>
     <row r="55">
       <c r="A55" s="261" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="B55" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C55" s="256" t="s">
         <v>1758</v>
@@ -71399,7 +71396,7 @@
       </c>
       <c r="E55" s="262"/>
       <c r="F55" s="128" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="G55" s="262"/>
       <c r="H55" s="262"/>
@@ -71425,10 +71422,10 @@
     </row>
     <row r="56">
       <c r="A56" s="261" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="B56" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C56" s="256" t="s">
         <v>1758</v>
@@ -71438,7 +71435,7 @@
       </c>
       <c r="E56" s="262"/>
       <c r="F56" s="255" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G56" s="262"/>
       <c r="H56" s="262"/>
@@ -71464,10 +71461,10 @@
     </row>
     <row r="57">
       <c r="A57" s="261" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="B57" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C57" s="256" t="s">
         <v>286</v>
@@ -71477,7 +71474,7 @@
       </c>
       <c r="E57" s="262"/>
       <c r="F57" s="255" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="G57" s="262"/>
       <c r="H57" s="262"/>
@@ -71501,10 +71498,10 @@
     </row>
     <row r="58">
       <c r="A58" s="261" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="B58" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C58" s="256" t="s">
         <v>286</v>
@@ -71514,7 +71511,7 @@
       </c>
       <c r="E58" s="262"/>
       <c r="F58" s="255" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="G58" s="262"/>
       <c r="H58" s="262"/>
@@ -71538,10 +71535,10 @@
     </row>
     <row r="59">
       <c r="A59" s="261" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="B59" s="127" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C59" s="256" t="s">
         <v>286</v>
@@ -71551,7 +71548,7 @@
       </c>
       <c r="E59" s="262"/>
       <c r="F59" s="255" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="G59" s="262"/>
       <c r="H59" s="262"/>
@@ -71575,13 +71572,13 @@
     </row>
     <row r="60">
       <c r="A60" s="261" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="B60" s="127" t="s">
         <v>266</v>
       </c>
       <c r="C60" s="256" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="D60" s="256">
         <v>1.0</v>
@@ -71614,13 +71611,13 @@
     </row>
     <row r="61">
       <c r="A61" s="261" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="B61" s="127" t="s">
         <v>266</v>
       </c>
       <c r="C61" s="256" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="D61" s="256">
         <v>1.0</v>
@@ -71653,7 +71650,7 @@
     </row>
     <row r="62">
       <c r="A62" s="261" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="B62" s="127" t="s">
         <v>266</v>
@@ -71666,7 +71663,7 @@
       </c>
       <c r="E62" s="262"/>
       <c r="F62" s="255" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="G62" s="262"/>
       <c r="H62" s="262"/>
@@ -71690,7 +71687,7 @@
     </row>
     <row r="63">
       <c r="A63" s="261" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="B63" s="127" t="s">
         <v>266</v>
@@ -71703,7 +71700,7 @@
       </c>
       <c r="E63" s="262"/>
       <c r="F63" s="255" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="G63" s="262"/>
       <c r="H63" s="262"/>
@@ -71727,7 +71724,7 @@
     </row>
     <row r="64">
       <c r="A64" s="261" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="B64" s="127" t="s">
         <v>266</v>
@@ -71740,7 +71737,7 @@
       </c>
       <c r="E64" s="262"/>
       <c r="F64" s="255" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="G64" s="262"/>
       <c r="H64" s="262"/>
@@ -71764,7 +71761,7 @@
     </row>
     <row r="65">
       <c r="A65" s="261" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="B65" s="127" t="s">
         <v>266</v>
@@ -71777,7 +71774,7 @@
       </c>
       <c r="E65" s="262"/>
       <c r="F65" s="255" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="G65" s="262"/>
       <c r="H65" s="262"/>
@@ -71801,7 +71798,7 @@
     </row>
     <row r="66">
       <c r="A66" s="261" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="B66" s="127" t="s">
         <v>266</v>
@@ -71814,7 +71811,7 @@
       </c>
       <c r="E66" s="262"/>
       <c r="F66" s="255" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="G66" s="262"/>
       <c r="H66" s="262"/>
@@ -71838,7 +71835,7 @@
     </row>
     <row r="67">
       <c r="A67" s="261" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="B67" s="127" t="s">
         <v>266</v>
@@ -71851,7 +71848,7 @@
       </c>
       <c r="E67" s="262"/>
       <c r="F67" s="255" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="G67" s="262"/>
       <c r="H67" s="262"/>
@@ -71875,7 +71872,7 @@
     </row>
     <row r="68">
       <c r="A68" s="261" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="B68" s="127" t="s">
         <v>266</v>
@@ -71888,7 +71885,7 @@
       </c>
       <c r="E68" s="262"/>
       <c r="F68" s="255" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="G68" s="262"/>
       <c r="H68" s="262"/>
@@ -71912,7 +71909,7 @@
     </row>
     <row r="69">
       <c r="A69" s="261" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="B69" s="127" t="s">
         <v>266</v>
@@ -71925,7 +71922,7 @@
       </c>
       <c r="E69" s="262"/>
       <c r="F69" s="255" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="G69" s="262"/>
       <c r="H69" s="262"/>
@@ -71949,7 +71946,7 @@
     </row>
     <row r="70">
       <c r="A70" s="261" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="B70" s="127" t="s">
         <v>266</v>
@@ -71962,7 +71959,7 @@
       </c>
       <c r="E70" s="262"/>
       <c r="F70" s="255" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="G70" s="262"/>
       <c r="H70" s="262"/>
@@ -71986,7 +71983,7 @@
     </row>
     <row r="71">
       <c r="A71" s="261" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="B71" s="127" t="s">
         <v>266</v>
@@ -71999,7 +71996,7 @@
       </c>
       <c r="E71" s="262"/>
       <c r="F71" s="255" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="G71" s="262"/>
       <c r="H71" s="262"/>
@@ -72023,7 +72020,7 @@
     </row>
     <row r="72">
       <c r="A72" s="261" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="B72" s="127" t="s">
         <v>266</v>
@@ -72036,7 +72033,7 @@
       </c>
       <c r="E72" s="262"/>
       <c r="F72" s="255" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="G72" s="262"/>
       <c r="H72" s="262"/>
@@ -72060,7 +72057,7 @@
     </row>
     <row r="73">
       <c r="A73" s="261" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="B73" s="127" t="s">
         <v>266</v>
@@ -72073,7 +72070,7 @@
       </c>
       <c r="E73" s="262"/>
       <c r="F73" s="255" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="G73" s="262"/>
       <c r="H73" s="262"/>
@@ -72097,7 +72094,7 @@
     </row>
     <row r="74">
       <c r="A74" s="261" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="B74" s="127" t="s">
         <v>266</v>
@@ -72110,7 +72107,7 @@
       </c>
       <c r="E74" s="262"/>
       <c r="F74" s="255" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="G74" s="262"/>
       <c r="H74" s="262"/>
@@ -72134,7 +72131,7 @@
     </row>
     <row r="75">
       <c r="A75" s="261" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="B75" s="127" t="s">
         <v>266</v>
@@ -72147,7 +72144,7 @@
       </c>
       <c r="E75" s="262"/>
       <c r="F75" s="255" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="G75" s="262"/>
       <c r="H75" s="262"/>
@@ -72171,7 +72168,7 @@
     </row>
     <row r="76">
       <c r="A76" s="261" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="B76" s="127" t="s">
         <v>266</v>
@@ -72184,7 +72181,7 @@
       </c>
       <c r="E76" s="268"/>
       <c r="F76" s="255" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="G76" s="268"/>
       <c r="H76" s="268"/>
@@ -72208,7 +72205,7 @@
     </row>
     <row r="77">
       <c r="A77" s="261" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="B77" s="127" t="s">
         <v>266</v>
@@ -72221,7 +72218,7 @@
       </c>
       <c r="E77" s="268"/>
       <c r="F77" s="255" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="G77" s="268"/>
       <c r="H77" s="268"/>
@@ -72245,7 +72242,7 @@
     </row>
     <row r="78">
       <c r="A78" s="261" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="B78" s="127" t="s">
         <v>266</v>
@@ -72258,7 +72255,7 @@
       </c>
       <c r="E78" s="268"/>
       <c r="F78" s="255" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
       <c r="G78" s="268"/>
       <c r="H78" s="268"/>
@@ -72282,7 +72279,7 @@
     </row>
     <row r="79">
       <c r="A79" s="261" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="B79" s="127" t="s">
         <v>266</v>
@@ -72295,7 +72292,7 @@
       </c>
       <c r="E79" s="268"/>
       <c r="F79" s="255" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
       <c r="G79" s="268"/>
       <c r="H79" s="268"/>
@@ -72319,7 +72316,7 @@
     </row>
     <row r="80">
       <c r="A80" s="261" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
       <c r="B80" s="127" t="s">
         <v>266</v>
@@ -72332,7 +72329,7 @@
       </c>
       <c r="E80" s="268"/>
       <c r="F80" s="255" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
       <c r="G80" s="268"/>
       <c r="H80" s="268"/>
@@ -72356,7 +72353,7 @@
     </row>
     <row r="81">
       <c r="A81" s="261" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="B81" s="127" t="s">
         <v>266</v>
@@ -72369,7 +72366,7 @@
       </c>
       <c r="E81" s="268"/>
       <c r="F81" s="255" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="G81" s="268"/>
       <c r="H81" s="268"/>
@@ -72393,7 +72390,7 @@
     </row>
     <row r="82">
       <c r="A82" s="261" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
       <c r="B82" s="127" t="s">
         <v>266</v>
@@ -72406,7 +72403,7 @@
       </c>
       <c r="E82" s="262"/>
       <c r="F82" s="255" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="G82" s="262"/>
       <c r="H82" s="262"/>
@@ -72430,7 +72427,7 @@
     </row>
     <row r="83">
       <c r="A83" s="261" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="B83" s="127" t="s">
         <v>266</v>
@@ -72443,7 +72440,7 @@
       </c>
       <c r="E83" s="262"/>
       <c r="F83" s="255" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
       <c r="G83" s="262"/>
       <c r="H83" s="262"/>
@@ -72467,7 +72464,7 @@
     </row>
     <row r="84">
       <c r="A84" s="261" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
       <c r="B84" s="127" t="s">
         <v>266</v>
@@ -72480,7 +72477,7 @@
       </c>
       <c r="E84" s="262"/>
       <c r="F84" s="255" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
       <c r="G84" s="262"/>
       <c r="H84" s="262"/>
@@ -72504,7 +72501,7 @@
     </row>
     <row r="85">
       <c r="A85" s="261" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
       <c r="B85" s="127" t="s">
         <v>266</v>
@@ -72517,7 +72514,7 @@
       </c>
       <c r="E85" s="262"/>
       <c r="F85" s="255" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
       <c r="G85" s="262"/>
       <c r="H85" s="262"/>
@@ -72541,7 +72538,7 @@
     </row>
     <row r="86">
       <c r="A86" s="261" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="B86" s="127" t="s">
         <v>266</v>
@@ -72554,7 +72551,7 @@
       </c>
       <c r="E86" s="262"/>
       <c r="F86" s="255" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="G86" s="262"/>
       <c r="H86" s="262"/>
@@ -72578,7 +72575,7 @@
     </row>
     <row r="87">
       <c r="A87" s="261" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="B87" s="127" t="s">
         <v>266</v>
@@ -72591,7 +72588,7 @@
       </c>
       <c r="E87" s="268"/>
       <c r="F87" s="255" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
       <c r="G87" s="268"/>
       <c r="H87" s="268"/>
@@ -72615,7 +72612,7 @@
     </row>
     <row r="88">
       <c r="A88" s="261" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="B88" s="127" t="s">
         <v>266</v>
@@ -72628,7 +72625,7 @@
       </c>
       <c r="E88" s="268"/>
       <c r="F88" s="255" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="G88" s="268"/>
       <c r="H88" s="268"/>
@@ -72652,7 +72649,7 @@
     </row>
     <row r="89">
       <c r="A89" s="261" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="B89" s="127" t="s">
         <v>266</v>
@@ -72665,7 +72662,7 @@
       </c>
       <c r="E89" s="268"/>
       <c r="F89" s="255" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
       <c r="G89" s="268"/>
       <c r="H89" s="268"/>
@@ -72689,7 +72686,7 @@
     </row>
     <row r="90">
       <c r="A90" s="261" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
       <c r="B90" s="127" t="s">
         <v>266</v>
@@ -72702,7 +72699,7 @@
       </c>
       <c r="E90" s="268"/>
       <c r="F90" s="255" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
       <c r="G90" s="268"/>
       <c r="H90" s="268"/>
@@ -72726,7 +72723,7 @@
     </row>
     <row r="91">
       <c r="A91" s="261" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
       <c r="B91" s="127" t="s">
         <v>266</v>
@@ -72739,7 +72736,7 @@
       </c>
       <c r="E91" s="268"/>
       <c r="F91" s="255" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="G91" s="268"/>
       <c r="H91" s="268"/>
@@ -72763,7 +72760,7 @@
     </row>
     <row r="92">
       <c r="A92" s="261" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="B92" s="127" t="s">
         <v>266</v>
@@ -72776,7 +72773,7 @@
       </c>
       <c r="E92" s="268"/>
       <c r="F92" s="255" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="G92" s="268"/>
       <c r="H92" s="268"/>
@@ -72800,7 +72797,7 @@
     </row>
     <row r="93">
       <c r="A93" s="261" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="B93" s="127" t="s">
         <v>266</v>
@@ -72813,7 +72810,7 @@
       </c>
       <c r="E93" s="262"/>
       <c r="F93" s="255" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
       <c r="G93" s="262"/>
       <c r="H93" s="262"/>
@@ -72837,7 +72834,7 @@
     </row>
     <row r="94">
       <c r="A94" s="261" t="s">
-        <v>2686</v>
+        <v>2685</v>
       </c>
       <c r="B94" s="127" t="s">
         <v>266</v>
@@ -72849,10 +72846,10 @@
         <v>1.0</v>
       </c>
       <c r="E94" s="269" t="s">
+        <v>2686</v>
+      </c>
+      <c r="F94" s="255" t="s">
         <v>2687</v>
-      </c>
-      <c r="F94" s="255" t="s">
-        <v>2688</v>
       </c>
       <c r="G94" s="262"/>
       <c r="H94" s="269">

</xml_diff>